<commit_message>
PDFs Fluxograma e GMUD
</commit_message>
<xml_diff>
--- a/Sprint 03/Atividade GMUD - 1ADSB Grupo 11 .xlsx
+++ b/Sprint 03/Atividade GMUD - 1ADSB Grupo 11 .xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Danilo\Documents\Projeto WINE GUARD\Wine-Guard\Sprint 03\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{551BCC01-B6F4-4A2D-A50E-04EDCDFEBECB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98FA94CE-8BAF-498D-9E3E-987D9751FB1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -324,7 +324,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
   <fonts count="14" x14ac:knownFonts="1">
     <font>
@@ -569,9 +569,41 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -587,7 +619,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -597,41 +628,10 @@
     <xf numFmtId="14" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hiperlink Visitado" xfId="2" builtinId="9" hidden="1"/>
@@ -935,9 +935,9 @@
   </sheetPr>
   <dimension ref="A1:J32"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E38" sqref="E38"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -968,12 +968,12 @@
       <c r="B2" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="21"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="33"/>
       <c r="G2" s="9" t="s">
         <v>26</v>
       </c>
@@ -985,12 +985,12 @@
       <c r="B3" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="17" t="s">
+      <c r="C3" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
       <c r="G3" s="10" t="s">
         <v>25</v>
       </c>
@@ -1002,12 +1002,12 @@
       <c r="B4" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
-      <c r="F4" s="24"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
       <c r="G4" s="10" t="s">
         <v>15</v>
       </c>
@@ -1016,29 +1016,29 @@
       </c>
     </row>
     <row r="6" spans="1:10" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="27" t="s">
+      <c r="B6" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="28"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="28"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="28"/>
-      <c r="H6" s="28"/>
+      <c r="C6" s="38"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="38"/>
+      <c r="G6" s="38"/>
+      <c r="H6" s="38"/>
     </row>
     <row r="7" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="16" t="s">
+      <c r="C7" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="22"/>
-      <c r="G7" s="22"/>
-      <c r="H7" s="22"/>
+      <c r="D7" s="26"/>
+      <c r="E7" s="26"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="26"/>
       <c r="J7" s="12"/>
     </row>
     <row r="8" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.25">
@@ -1046,421 +1046,421 @@
       <c r="B8" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="22"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="22"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="22"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="26"/>
     </row>
     <row r="9" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="C9" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="22"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="22"/>
+      <c r="D9" s="26"/>
+      <c r="E9" s="26"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="26"/>
     </row>
     <row r="10" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="16" t="s">
+      <c r="C10" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="22"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="22"/>
-      <c r="H10" s="22"/>
+      <c r="D10" s="26"/>
+      <c r="E10" s="26"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="26"/>
     </row>
     <row r="11" spans="1:10" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="23" t="s">
+      <c r="C11" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="D11" s="22"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="22"/>
-      <c r="H11" s="22"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="26"/>
+      <c r="H11" s="26"/>
     </row>
     <row r="12" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="23" t="s">
+      <c r="C12" s="34" t="s">
         <v>33</v>
       </c>
-      <c r="D12" s="16"/>
-      <c r="E12" s="16"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="16"/>
-      <c r="H12" s="16"/>
+      <c r="D12" s="25"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="25"/>
     </row>
     <row r="13" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C13" s="16" t="s">
+      <c r="C13" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="22"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="22"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="22"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="26"/>
+      <c r="H13" s="26"/>
     </row>
     <row r="14" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="16" t="s">
+      <c r="C14" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="22"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="22"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="22"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="26"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="26"/>
+      <c r="H14" s="26"/>
     </row>
     <row r="15" spans="1:10" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="16" t="s">
+      <c r="C15" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="D15" s="22"/>
-      <c r="E15" s="22"/>
-      <c r="F15" s="22"/>
-      <c r="G15" s="22"/>
-      <c r="H15" s="22"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="26"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="26"/>
+      <c r="H15" s="26"/>
     </row>
     <row r="16" spans="1:10" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="27" t="s">
+      <c r="B16" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="C16" s="28"/>
-      <c r="D16" s="28"/>
-      <c r="E16" s="28"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="28"/>
-      <c r="H16" s="28"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="38"/>
+      <c r="E16" s="38"/>
+      <c r="F16" s="38"/>
+      <c r="G16" s="38"/>
+      <c r="H16" s="38"/>
     </row>
     <row r="17" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
-      <c r="B17" s="29" t="s">
+      <c r="B17" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="C17" s="26"/>
-      <c r="D17" s="25" t="s">
+      <c r="C17" s="28"/>
+      <c r="D17" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="E17" s="22"/>
+      <c r="E17" s="26"/>
       <c r="F17" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="G17" s="25" t="s">
+      <c r="G17" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="H17" s="22"/>
+      <c r="H17" s="26"/>
     </row>
     <row r="19" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3"/>
-      <c r="B19" s="30" t="s">
+      <c r="B19" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="C19" s="30"/>
-      <c r="D19" s="30"/>
-      <c r="E19" s="30"/>
-      <c r="F19" s="30"/>
-      <c r="G19" s="30"/>
-      <c r="H19" s="30"/>
-      <c r="I19" s="30"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="21"/>
+      <c r="H19" s="21"/>
+      <c r="I19" s="21"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B20" s="31" t="s">
+      <c r="B20" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="C20" s="31" t="s">
+      <c r="C20" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="D20" s="31" t="s">
+      <c r="D20" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="E20" s="31" t="s">
+      <c r="E20" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="F20" s="31"/>
-      <c r="G20" s="31" t="s">
+      <c r="F20" s="16"/>
+      <c r="G20" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="H20" s="32" t="s">
+      <c r="H20" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="I20" s="31" t="s">
+      <c r="I20" s="16" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B21" s="33" t="s">
+    <row r="21" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="C21" s="34">
+      <c r="C21" s="19">
         <v>0.95833333333333337</v>
       </c>
-      <c r="D21" s="34">
+      <c r="D21" s="19">
         <v>0.96875</v>
       </c>
-      <c r="E21" s="33" t="s">
+      <c r="E21" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="F21" s="33"/>
-      <c r="G21" s="33" t="s">
+      <c r="F21" s="18"/>
+      <c r="G21" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="H21" s="35" t="s">
+      <c r="H21" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="I21" s="33" t="s">
+      <c r="I21" s="18" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B22" s="33" t="s">
+    <row r="22" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="C22" s="34">
+      <c r="C22" s="19">
         <v>0.96875</v>
       </c>
-      <c r="D22" s="34">
+      <c r="D22" s="19">
         <v>0.99305555555555558</v>
       </c>
-      <c r="E22" s="33" t="s">
+      <c r="E22" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="F22" s="33"/>
-      <c r="G22" s="33" t="s">
+      <c r="F22" s="18"/>
+      <c r="G22" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="H22" s="35" t="s">
+      <c r="H22" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="I22" s="33" t="s">
+      <c r="I22" s="18" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B23" s="33" t="s">
+    <row r="23" spans="1:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="C23" s="34">
+      <c r="C23" s="19">
         <v>0.99305555555555558</v>
       </c>
-      <c r="D23" s="34">
+      <c r="D23" s="19">
         <v>6.9444444444444441E-3</v>
       </c>
-      <c r="E23" s="33" t="s">
+      <c r="E23" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="F23" s="33"/>
-      <c r="G23" s="33" t="s">
+      <c r="F23" s="18"/>
+      <c r="G23" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="H23" s="35" t="s">
+      <c r="H23" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="I23" s="33" t="s">
+      <c r="I23" s="18" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="27" x14ac:dyDescent="0.25">
-      <c r="B24" s="33" t="s">
+      <c r="B24" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="C24" s="34">
+      <c r="C24" s="19">
         <v>6.9444444444444441E-3</v>
       </c>
-      <c r="D24" s="34">
+      <c r="D24" s="19">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="E24" s="33" t="s">
+      <c r="E24" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="F24" s="33"/>
-      <c r="G24" s="33" t="s">
+      <c r="F24" s="18"/>
+      <c r="G24" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="H24" s="35" t="s">
+      <c r="H24" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="I24" s="33" t="s">
+      <c r="I24" s="18" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B25" s="33" t="s">
+    <row r="25" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="18" t="s">
         <v>49</v>
       </c>
-      <c r="C25" s="34">
+      <c r="C25" s="19">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="D25" s="34">
+      <c r="D25" s="19">
         <v>4.8611111111111112E-2</v>
       </c>
-      <c r="E25" s="33" t="s">
+      <c r="E25" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="F25" s="33"/>
-      <c r="G25" s="33" t="s">
+      <c r="F25" s="18"/>
+      <c r="G25" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="H25" s="35" t="s">
+      <c r="H25" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="I25" s="33" t="s">
+      <c r="I25" s="18" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B26" s="33" t="s">
+    <row r="26" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="C26" s="34">
+      <c r="C26" s="19">
         <v>4.8611111111111112E-2</v>
       </c>
-      <c r="D26" s="34">
+      <c r="D26" s="19">
         <v>6.9444444444444448E-2</v>
       </c>
-      <c r="E26" s="33" t="s">
+      <c r="E26" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="F26" s="33"/>
-      <c r="G26" s="33" t="s">
+      <c r="F26" s="18"/>
+      <c r="G26" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="H26" s="35" t="s">
+      <c r="H26" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="I26" s="33" t="s">
+      <c r="I26" s="18" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B27" s="33" t="s">
+    <row r="27" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="C27" s="34">
+      <c r="C27" s="19">
         <v>6.9444444444444448E-2</v>
       </c>
-      <c r="D27" s="34">
+      <c r="D27" s="19">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="E27" s="33" t="s">
+      <c r="E27" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="F27" s="33"/>
-      <c r="G27" s="33" t="s">
+      <c r="F27" s="18"/>
+      <c r="G27" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="H27" s="35" t="s">
+      <c r="H27" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="I27" s="33" t="s">
+      <c r="I27" s="18" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B28" s="33" t="s">
+    <row r="28" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="C28" s="34">
+      <c r="C28" s="19">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="D28" s="34">
+      <c r="D28" s="19">
         <v>0.10416666666666667</v>
       </c>
-      <c r="E28" s="33" t="s">
+      <c r="E28" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="F28" s="33"/>
-      <c r="G28" s="33" t="s">
+      <c r="F28" s="18"/>
+      <c r="G28" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="H28" s="35" t="s">
+      <c r="H28" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="I28" s="33" t="s">
+      <c r="I28" s="18" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3"/>
-      <c r="B29" s="36" t="s">
+      <c r="B29" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="C29" s="37"/>
-      <c r="D29" s="37"/>
-      <c r="E29" s="37"/>
-      <c r="F29" s="37"/>
-      <c r="G29" s="37"/>
-      <c r="H29" s="37"/>
-      <c r="I29" s="37"/>
+      <c r="C29" s="23"/>
+      <c r="D29" s="23"/>
+      <c r="E29" s="23"/>
+      <c r="F29" s="23"/>
+      <c r="G29" s="23"/>
+      <c r="H29" s="23"/>
+      <c r="I29" s="23"/>
     </row>
     <row r="30" spans="1:9" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3"/>
-      <c r="B30" s="38" t="s">
+      <c r="B30" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="C30" s="38"/>
-      <c r="D30" s="38"/>
-      <c r="E30" s="38"/>
-      <c r="F30" s="38"/>
-      <c r="G30" s="38"/>
-      <c r="H30" s="38"/>
-      <c r="I30" s="38"/>
+      <c r="C30" s="24"/>
+      <c r="D30" s="24"/>
+      <c r="E30" s="24"/>
+      <c r="F30" s="24"/>
+      <c r="G30" s="24"/>
+      <c r="H30" s="24"/>
+      <c r="I30" s="24"/>
     </row>
     <row r="31" spans="1:9" ht="8.1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="32" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="C8:H8"/>
+    <mergeCell ref="C3:F3"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="C15:H15"/>
+    <mergeCell ref="C12:H12"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="C11:H11"/>
+    <mergeCell ref="C13:H13"/>
+    <mergeCell ref="B6:H6"/>
+    <mergeCell ref="C9:H9"/>
+    <mergeCell ref="C7:H7"/>
     <mergeCell ref="B19:I19"/>
     <mergeCell ref="B29:I29"/>
     <mergeCell ref="B30:I30"/>
     <mergeCell ref="C10:H10"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="C14:H14"/>
-    <mergeCell ref="C8:H8"/>
-    <mergeCell ref="C3:F3"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="C15:H15"/>
-    <mergeCell ref="C12:H12"/>
-    <mergeCell ref="C4:F4"/>
     <mergeCell ref="G17:H17"/>
-    <mergeCell ref="C11:H11"/>
-    <mergeCell ref="C13:H13"/>
     <mergeCell ref="D17:E17"/>
     <mergeCell ref="B16:H16"/>
-    <mergeCell ref="B6:H6"/>
-    <mergeCell ref="C9:H9"/>
-    <mergeCell ref="C7:H7"/>
   </mergeCells>
   <conditionalFormatting sqref="C21:D21">
     <cfRule type="timePeriod" dxfId="0" priority="1" timePeriod="lastMonth">

</xml_diff>